<commit_message>
update blog for fuel allocation
</commit_message>
<xml_diff>
--- a/PM-Post.xlsx
+++ b/PM-Post.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minxing/Project/EnviroByte/Website/EnviroByte-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD2D6F8D-B122-8844-8AE3-58B07EF1F09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A95A3-D492-794E-BD08-6DC635206B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="2660" windowWidth="27240" windowHeight="16440" xr2:uid="{DE95740A-E51D-AC4B-8C3B-27002BE8F9BD}"/>
+    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17260" xr2:uid="{DE95740A-E51D-AC4B-8C3B-27002BE8F9BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -119,7 +119,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -151,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,16 +159,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -507,7 +524,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,124 +597,128 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>24140</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="4" t="str">
         <f>IF(B10&gt;B6,"Yes","No")</f>
         <v>No</v>
       </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>43504</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="4" t="str">
         <f t="shared" ref="C11:C15" si="0">IF(B11&gt;B7,"Yes","No")</f>
         <v>Yes</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>79236</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>43356</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>50674</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>60445</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="5">
         <v>1000000</v>
       </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">

</xml_diff>